<commit_message>
tp procesos e hilos 2 arreglado
</commit_message>
<xml_diff>
--- a/Clases Jueves/TP 2/Ejercicio 7.xlsx
+++ b/Clases Jueves/TP 2/Ejercicio 7.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\54344\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\UADER\Tercero\Sistemas operativos\Clases Jueves\TP 2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{950BB554-1E50-42A0-8826-673940374C13}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{91CC36DD-9F0E-4932-8F59-C4F83B93A243}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10560" xr2:uid="{6A0D0AB2-8D01-4B02-BB79-8E4077938BC9}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t>P1</t>
   </si>
@@ -45,12 +45,21 @@
   <si>
     <t>P3</t>
   </si>
+  <si>
+    <t>LISTO</t>
+  </si>
+  <si>
+    <t>DETENIDO</t>
+  </si>
+  <si>
+    <t>EJECUCION</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -66,8 +75,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="9"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="9">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -94,25 +110,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.59999389629810485"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.59999389629810485"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="-0.249977111117893"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.39997558519241921"/>
+        <fgColor rgb="FFC00000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -144,7 +142,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -153,12 +151,21 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -475,8 +482,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{14EF95FB-3B48-4C61-854F-3EBC84B5E612}">
   <dimension ref="A1:Z7"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="AB10" sqref="AB10"/>
+    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -492,23 +499,23 @@
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="2"/>
-      <c r="C1" s="2"/>
-      <c r="D1" s="2"/>
-      <c r="E1" s="2"/>
-      <c r="F1" s="2"/>
-      <c r="G1" s="2"/>
-      <c r="H1" s="2"/>
-      <c r="I1" s="2"/>
-      <c r="J1" s="5"/>
-      <c r="K1" s="5"/>
-      <c r="L1" s="5"/>
-      <c r="M1" s="5"/>
-      <c r="N1" s="2"/>
-      <c r="O1" s="2"/>
-      <c r="P1" s="2"/>
-      <c r="Q1" s="2"/>
-      <c r="R1" s="5"/>
+      <c r="B1" s="5"/>
+      <c r="C1" s="5"/>
+      <c r="D1" s="5"/>
+      <c r="E1" s="5"/>
+      <c r="F1" s="5"/>
+      <c r="G1" s="5"/>
+      <c r="H1" s="5"/>
+      <c r="I1" s="5"/>
+      <c r="J1" s="4"/>
+      <c r="K1" s="4"/>
+      <c r="L1" s="4"/>
+      <c r="M1" s="4"/>
+      <c r="N1" s="5"/>
+      <c r="O1" s="5"/>
+      <c r="P1" s="5"/>
+      <c r="Q1" s="5"/>
+      <c r="R1" s="4"/>
       <c r="S1" s="2"/>
       <c r="T1" s="2"/>
       <c r="U1" s="2"/>
@@ -522,29 +529,29 @@
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="2"/>
-      <c r="C2" s="2"/>
-      <c r="D2" s="2"/>
-      <c r="E2" s="2"/>
-      <c r="F2" s="6"/>
-      <c r="G2" s="6"/>
-      <c r="H2" s="6"/>
-      <c r="I2" s="6"/>
-      <c r="J2" s="2"/>
-      <c r="K2" s="2"/>
-      <c r="L2" s="2"/>
-      <c r="M2" s="2"/>
-      <c r="N2" s="2"/>
-      <c r="O2" s="2"/>
-      <c r="P2" s="2"/>
-      <c r="Q2" s="6"/>
-      <c r="R2" s="6"/>
-      <c r="S2" s="9"/>
-      <c r="T2" s="9"/>
-      <c r="U2" s="9"/>
-      <c r="V2" s="9"/>
-      <c r="W2" s="10"/>
-      <c r="X2" s="10"/>
+      <c r="B2" s="5"/>
+      <c r="C2" s="5"/>
+      <c r="D2" s="5"/>
+      <c r="E2" s="5"/>
+      <c r="F2" s="4"/>
+      <c r="G2" s="4"/>
+      <c r="H2" s="4"/>
+      <c r="I2" s="4"/>
+      <c r="J2" s="5"/>
+      <c r="K2" s="5"/>
+      <c r="L2" s="5"/>
+      <c r="M2" s="5"/>
+      <c r="N2" s="5"/>
+      <c r="O2" s="5"/>
+      <c r="P2" s="5"/>
+      <c r="Q2" s="4"/>
+      <c r="R2" s="4"/>
+      <c r="S2" s="8"/>
+      <c r="T2" s="8"/>
+      <c r="U2" s="8"/>
+      <c r="V2" s="8"/>
+      <c r="W2" s="4"/>
+      <c r="X2" s="4"/>
       <c r="Y2" s="2"/>
       <c r="Z2" s="2"/>
     </row>
@@ -556,17 +563,17 @@
       <c r="C3" s="4"/>
       <c r="D3" s="4"/>
       <c r="E3" s="4"/>
-      <c r="F3" s="2"/>
-      <c r="G3" s="2"/>
-      <c r="H3" s="2"/>
-      <c r="I3" s="2"/>
-      <c r="J3" s="2"/>
-      <c r="K3" s="2"/>
-      <c r="L3" s="2"/>
-      <c r="M3" s="2"/>
-      <c r="N3" s="8"/>
-      <c r="O3" s="8"/>
-      <c r="P3" s="8"/>
+      <c r="F3" s="5"/>
+      <c r="G3" s="5"/>
+      <c r="H3" s="5"/>
+      <c r="I3" s="5"/>
+      <c r="J3" s="5"/>
+      <c r="K3" s="5"/>
+      <c r="L3" s="5"/>
+      <c r="M3" s="5"/>
+      <c r="N3" s="4"/>
+      <c r="O3" s="4"/>
+      <c r="P3" s="4"/>
       <c r="Q3" s="2"/>
       <c r="R3" s="2"/>
       <c r="S3" s="2"/>
@@ -580,86 +587,113 @@
     </row>
     <row r="4" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A4" s="3"/>
-      <c r="B4" s="2">
+      <c r="B4" s="13">
         <v>4</v>
       </c>
-      <c r="C4" s="2">
+      <c r="C4" s="13">
         <v>8</v>
       </c>
-      <c r="D4" s="2">
+      <c r="D4" s="13">
         <v>12</v>
       </c>
-      <c r="E4" s="2">
+      <c r="E4" s="13">
         <v>16</v>
       </c>
-      <c r="F4" s="2">
+      <c r="F4" s="13">
         <v>20</v>
       </c>
-      <c r="G4" s="2">
+      <c r="G4" s="13">
         <v>24</v>
       </c>
-      <c r="H4" s="2">
+      <c r="H4" s="13">
         <v>28</v>
       </c>
-      <c r="I4" s="2">
+      <c r="I4" s="13">
         <v>32</v>
       </c>
-      <c r="J4" s="2">
+      <c r="J4" s="13">
         <v>36</v>
       </c>
-      <c r="K4" s="2">
+      <c r="K4" s="13">
         <v>40</v>
       </c>
-      <c r="L4" s="2">
+      <c r="L4" s="13">
         <v>44</v>
       </c>
-      <c r="M4" s="2">
+      <c r="M4" s="13">
         <v>48</v>
       </c>
-      <c r="N4" s="2">
+      <c r="N4" s="13">
         <v>52</v>
       </c>
-      <c r="O4" s="2">
+      <c r="O4" s="13">
         <v>56</v>
       </c>
-      <c r="P4" s="2">
+      <c r="P4" s="13">
         <v>60</v>
       </c>
-      <c r="Q4" s="7">
+      <c r="Q4" s="14">
         <v>64</v>
       </c>
-      <c r="R4" s="7">
+      <c r="R4" s="14">
         <v>68</v>
       </c>
-      <c r="S4" s="7">
+      <c r="S4" s="14">
         <v>72</v>
       </c>
-      <c r="T4" s="7">
+      <c r="T4" s="14">
         <v>76</v>
       </c>
-      <c r="U4" s="7">
+      <c r="U4" s="14">
         <v>77</v>
       </c>
-      <c r="V4" s="7">
+      <c r="V4" s="14">
         <v>78</v>
       </c>
-      <c r="W4" s="7">
+      <c r="W4" s="14">
         <v>82</v>
       </c>
-      <c r="X4" s="7">
+      <c r="X4" s="14">
         <v>86</v>
       </c>
-      <c r="Y4" s="7">
+      <c r="Y4" s="14">
         <v>90</v>
       </c>
-      <c r="Z4" s="7">
+      <c r="Z4" s="14">
         <v>94</v>
       </c>
+    </row>
+    <row r="6" spans="1:26" x14ac:dyDescent="0.35">
+      <c r="B6" s="7"/>
+      <c r="C6" s="7"/>
+      <c r="E6" s="10"/>
+      <c r="F6" s="10"/>
+      <c r="H6" s="9"/>
+      <c r="I6" s="9"/>
+      <c r="J6" s="11"/>
     </row>
     <row r="7" spans="1:26" x14ac:dyDescent="0.35">
-      <c r="X7" s="11"/>
+      <c r="B7" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="C7" s="12"/>
+      <c r="E7" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="F7" s="12"/>
+      <c r="H7" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="I7" s="12"/>
+      <c r="X7" s="6"/>
     </row>
   </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="B7:C7"/>
+    <mergeCell ref="E7:F7"/>
+    <mergeCell ref="H7:I7"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>